<commit_message>
boost stats pre battle due to buffs
</commit_message>
<xml_diff>
--- a/app/data/buffs.xlsx
+++ b/app/data/buffs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>hp_base</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>grants the team bonus attack damage</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>No Title</t>
+  </si>
+  <si>
+    <t>grants the team nothing</t>
   </si>
 </sst>
 </file>
@@ -440,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,6 +792,53 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>